<commit_message>
andrea miele is now a PO
</commit_message>
<xml_diff>
--- a/static/results/2026_po.xlsx
+++ b/static/results/2026_po.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="111">
   <si>
     <t xml:space="preserve">Codice_meccanografico</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2008-12-29</t>
   </si>
 </sst>
 </file>
@@ -359,6 +368,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -444,20 +454,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.41"/>
@@ -1036,6 +1046,44 @@
         <v>107</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>